<commit_message>
changing pheno stage calculation to include just subset of 2023 data. recalculate other metrics. start safety margin calculation
</commit_message>
<xml_diff>
--- a/data/LT50 master.xlsx
+++ b/data/LT50 master.xlsx
@@ -740,7 +740,7 @@
         <v>4</v>
       </c>
       <c r="L8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M8">
         <v>537.65</v>
@@ -786,7 +786,7 @@
         <v>4</v>
       </c>
       <c r="L9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M9">
         <v>537.65</v>
@@ -832,7 +832,7 @@
         <v>4</v>
       </c>
       <c r="L10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M10">
         <v>537.65</v>
@@ -878,7 +878,7 @@
         <v>4</v>
       </c>
       <c r="L11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M11">
         <v>537.65</v>
@@ -924,7 +924,7 @@
         <v>4</v>
       </c>
       <c r="L12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M12">
         <v>537.65</v>
@@ -970,7 +970,7 @@
         <v>4</v>
       </c>
       <c r="L13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M13">
         <v>537.65</v>
@@ -3590,7 +3590,7 @@
         <v>5</v>
       </c>
       <c r="L68">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M68">
         <v>574</v>
@@ -3636,7 +3636,7 @@
         <v>5</v>
       </c>
       <c r="L69">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M69">
         <v>574</v>
@@ -3682,7 +3682,7 @@
         <v>5</v>
       </c>
       <c r="L70">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M70">
         <v>574</v>
@@ -3728,7 +3728,7 @@
         <v>5</v>
       </c>
       <c r="L71">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M71">
         <v>574</v>
@@ -3774,7 +3774,7 @@
         <v>5</v>
       </c>
       <c r="L72">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M72">
         <v>574</v>
@@ -3820,7 +3820,7 @@
         <v>5</v>
       </c>
       <c r="L73">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M73">
         <v>574</v>
@@ -7730,7 +7730,7 @@
         <v>3</v>
       </c>
       <c r="L158">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M158">
         <v>324.25</v>
@@ -7776,7 +7776,7 @@
         <v>3</v>
       </c>
       <c r="L159">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M159">
         <v>324.25</v>
@@ -7822,7 +7822,7 @@
         <v>3</v>
       </c>
       <c r="L160">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M160">
         <v>324.25</v>
@@ -7868,7 +7868,7 @@
         <v>3</v>
       </c>
       <c r="L161">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M161">
         <v>324.25</v>
@@ -7914,7 +7914,7 @@
         <v>3</v>
       </c>
       <c r="L162">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M162">
         <v>324.25</v>
@@ -7960,7 +7960,7 @@
         <v>3</v>
       </c>
       <c r="L163">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M163">
         <v>324.25</v>
@@ -8558,7 +8558,7 @@
         <v>3</v>
       </c>
       <c r="L176">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M176">
         <v>178.55</v>
@@ -8604,7 +8604,7 @@
         <v>3</v>
       </c>
       <c r="L177">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M177">
         <v>178.55</v>
@@ -8650,7 +8650,7 @@
         <v>3</v>
       </c>
       <c r="L178">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M178">
         <v>178.55</v>
@@ -8696,7 +8696,7 @@
         <v>3</v>
       </c>
       <c r="L179">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M179">
         <v>178.55</v>
@@ -8742,7 +8742,7 @@
         <v>3</v>
       </c>
       <c r="L180">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M180">
         <v>178.55</v>
@@ -8788,7 +8788,7 @@
         <v>3</v>
       </c>
       <c r="L181">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M181">
         <v>178.55</v>

</xml_diff>